<commit_message>
modifying the Semp end-use for scalar data
</commit_message>
<xml_diff>
--- a/Input/ScheduleSemp.xlsx
+++ b/Input/ScheduleSemp.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr15640\Desktop\EUReCA\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02FFCF6-5EC5-4FE8-86AF-2C1BB1553540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F510E2-5742-44B9-81E0-1680DC66A42A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{102ADA3B-B81C-C94C-911C-48E8DF6FFDE7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Residenziale" sheetId="2" r:id="rId1"/>
-    <sheet name="Terziario" sheetId="1" r:id="rId2"/>
-    <sheet name="Servizi" sheetId="5" r:id="rId3"/>
-    <sheet name="Commerciale" sheetId="9" r:id="rId4"/>
+    <sheet name="GeneralData" sheetId="10" r:id="rId1"/>
+    <sheet name="Residenziale" sheetId="2" r:id="rId2"/>
+    <sheet name="Terziario" sheetId="1" r:id="rId3"/>
+    <sheet name="Servizi" sheetId="5" r:id="rId4"/>
+    <sheet name="Commerciale" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="36">
   <si>
     <t>Weekday</t>
   </si>
@@ -98,6 +99,45 @@
   <si>
     <t>[g/(m² s)]</t>
   </si>
+  <si>
+    <t>Archetype list</t>
+  </si>
+  <si>
+    <t>[0-1]</t>
+  </si>
+  <si>
+    <t>[Bool]</t>
+  </si>
+  <si>
+    <t>ConvFrac</t>
+  </si>
+  <si>
+    <t>AHUHum</t>
+  </si>
+  <si>
+    <t>SensRec</t>
+  </si>
+  <si>
+    <t>LatRec</t>
+  </si>
+  <si>
+    <t>OutAirRatio</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Residenziale</t>
+  </si>
+  <si>
+    <t>Terziario</t>
+  </si>
+  <si>
+    <t>Servizi</t>
+  </si>
+  <si>
+    <t>Commerciale</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +182,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E0B4"/>
+        <bgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -573,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -669,6 +721,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,6 +741,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -702,6 +759,94 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CasellaDiTesto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A136A88-63A5-43BD-8E84-E070F94D9213}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5114925" y="171450"/>
+          <a:ext cx="3228975" cy="1200150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100"/>
+            <a:t>All archetypes listed here are loaded</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" baseline="0"/>
+            <a:t> (if </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" b="1" baseline="0"/>
+            <a:t>daily</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1100" baseline="0"/>
+            <a:t> archetype loading method is used)</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1000,11 +1145,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CB4D20-8171-4D3A-B436-C3966BA8F7D8}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>0.6</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>0.6</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>0.6</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>0.6</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEDE6AD-DD94-FE41-A4EE-7AF52AB62231}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1024,32 +1306,32 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
-      <c r="B1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="38"/>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="40"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -2977,7 +3259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836E031D-39EA-D045-9F49-CB54553714EE}">
   <dimension ref="A1:X28"/>
   <sheetViews>
@@ -3002,32 +3284,32 @@
   <sheetData>
     <row r="1" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
-      <c r="B1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="38"/>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="40"/>
       <c r="X1" s="14"/>
     </row>
     <row r="2" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4956,7 +5238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB3B609-DA64-6B46-9D4D-885AFA6B0260}">
   <dimension ref="A1:W28"/>
   <sheetViews>
@@ -4981,32 +5263,32 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
-      <c r="B1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="38"/>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="40"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -6935,7 +7217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75507A1-6ACA-4709-9C5A-80C8BCBF7953}">
   <dimension ref="A1:W28"/>
   <sheetViews>
@@ -6960,32 +7242,32 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
-      <c r="B1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="38"/>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="40"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">

</xml_diff>